<commit_message>
Refactor Excel table example: Improve sheet processing by grouping sheets by type while maintaining original order, enhance debug logging for sheet data analysis, and streamline data handling for sub-item details. Update SQL queries for clarity and efficiency.
</commit_message>
<xml_diff>
--- a/assets/excel/指标汇总.xlsx
+++ b/assets/excel/指标汇总.xlsx
@@ -4,11 +4,13 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="17240"/>
+    <workbookView windowHeight="16640" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="道路工程 主干路67cm m2" sheetId="1" r:id="rId1"/>
-    <sheet name="交通工程 次干路59cm m2" sheetId="2" r:id="rId2"/>
+    <sheet name="道路工程 主干路57cm m2" sheetId="3" r:id="rId2"/>
+    <sheet name="交通工程 次干路59cm m2" sheetId="2" r:id="rId3"/>
+    <sheet name="交通工程 次干路69cm m2" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029" iterate="1" iterateCount="100" iterateDelta="0.001"/>
   <extLst>
@@ -28,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="72">
   <si>
     <t>单位工程人材机汇总表</t>
   </si>
@@ -235,6 +237,9 @@
   </si>
   <si>
     <t>其他机具费</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
   <si>
     <t>合  计</t>
@@ -1426,20 +1431,21 @@
   <sheetPr/>
   <dimension ref="A1:I47"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="I32" sqref="A3:I32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.6"/>
   <cols>
     <col min="1" max="1" width="11.5" customWidth="1"/>
-    <col min="2" max="2" width="14.6590909090909" customWidth="1"/>
+    <col min="2" max="2" width="20.2613636363636" customWidth="1"/>
     <col min="3" max="3" width="10.5" customWidth="1"/>
-    <col min="4" max="4" width="20.1590909090909" customWidth="1"/>
-    <col min="5" max="5" width="9.82954545454546" customWidth="1"/>
+    <col min="4" max="4" width="28.7727272727273" customWidth="1"/>
+    <col min="5" max="5" width="16.0909090909091" customWidth="1"/>
     <col min="6" max="6" width="6.5" customWidth="1"/>
     <col min="7" max="7" width="7.82954545454545" customWidth="1"/>
-    <col min="8" max="9" width="14.3295454545455" customWidth="1"/>
+    <col min="8" max="8" width="14.3295454545455" customWidth="1"/>
+    <col min="9" max="9" width="26.125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="29.25" customHeight="1" spans="1:9">
@@ -2154,8 +2160,8 @@
       <c r="H32" s="13">
         <v>1</v>
       </c>
-      <c r="I32" s="17">
-        <v>0.36</v>
+      <c r="I32" s="17" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="33" ht="14.25" customHeight="1" spans="1:9">
@@ -2316,7 +2322,7 @@
       <c r="A47" s="8"/>
       <c r="B47" s="9"/>
       <c r="C47" s="9" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D47" s="9"/>
       <c r="E47" s="9"/>
@@ -2437,6 +2443,1017 @@
   <dimension ref="A1:I47"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="I32" sqref="A3:I32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.6"/>
+  <cols>
+    <col min="1" max="1" width="11.5" customWidth="1"/>
+    <col min="2" max="2" width="20.2613636363636" customWidth="1"/>
+    <col min="3" max="3" width="10.5" customWidth="1"/>
+    <col min="4" max="4" width="28.7727272727273" customWidth="1"/>
+    <col min="5" max="5" width="16.0909090909091" customWidth="1"/>
+    <col min="6" max="6" width="6.5" customWidth="1"/>
+    <col min="7" max="7" width="7.82954545454545" customWidth="1"/>
+    <col min="8" max="8" width="14.3295454545455" customWidth="1"/>
+    <col min="9" max="9" width="26.125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="29.25" customHeight="1" spans="1:9">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+    </row>
+    <row r="2" ht="28.5" customHeight="1" spans="1:9">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+    </row>
+    <row r="3" ht="14.25" customHeight="1" spans="1:9">
+      <c r="A3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I3" s="15" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" ht="14.25" customHeight="1" spans="1:9">
+      <c r="A4" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="7"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="16"/>
+    </row>
+    <row r="5" ht="14.25" customHeight="1" spans="1:9">
+      <c r="A5" s="6">
+        <v>1</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="7"/>
+      <c r="E5" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="13">
+        <v>0.1116</v>
+      </c>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13">
+        <v>118.5</v>
+      </c>
+      <c r="I5" s="17">
+        <v>13.22</v>
+      </c>
+    </row>
+    <row r="6" ht="14.25" customHeight="1" spans="1:9">
+      <c r="A6" s="6">
+        <v>2</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="7"/>
+      <c r="E6" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" s="13">
+        <v>-0.0003</v>
+      </c>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13">
+        <v>1</v>
+      </c>
+      <c r="I6" s="17"/>
+    </row>
+    <row r="7" ht="14.25" customHeight="1" spans="1:9">
+      <c r="A7" s="6"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="17"/>
+    </row>
+    <row r="8" ht="14.25" customHeight="1" spans="1:9">
+      <c r="A8" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="7"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="17"/>
+    </row>
+    <row r="9" ht="14.25" customHeight="1" spans="1:9">
+      <c r="A9" s="6">
+        <v>1</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="7"/>
+      <c r="E9" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="F9" s="13">
+        <v>0.0003</v>
+      </c>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13">
+        <v>1</v>
+      </c>
+      <c r="I9" s="17"/>
+    </row>
+    <row r="10" ht="14.25" customHeight="1" spans="1:9">
+      <c r="A10" s="6">
+        <v>2</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="7"/>
+      <c r="E10" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="F10" s="13">
+        <v>1.3671</v>
+      </c>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13">
+        <v>7.76</v>
+      </c>
+      <c r="I10" s="17">
+        <v>10.61</v>
+      </c>
+    </row>
+    <row r="11" ht="14.25" customHeight="1" spans="1:9">
+      <c r="A11" s="6">
+        <v>3</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" s="7"/>
+      <c r="E11" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="F11" s="13">
+        <v>0.0938</v>
+      </c>
+      <c r="G11" s="13"/>
+      <c r="H11" s="13">
+        <v>402.7</v>
+      </c>
+      <c r="I11" s="17">
+        <v>37.77</v>
+      </c>
+    </row>
+    <row r="12" ht="14.25" customHeight="1" spans="1:9">
+      <c r="A12" s="6">
+        <v>4</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" s="7"/>
+      <c r="E12" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="F12" s="13">
+        <v>0.1423</v>
+      </c>
+      <c r="G12" s="13"/>
+      <c r="H12" s="13">
+        <v>385</v>
+      </c>
+      <c r="I12" s="17">
+        <v>54.79</v>
+      </c>
+    </row>
+    <row r="13" ht="14.25" customHeight="1" spans="1:9">
+      <c r="A13" s="6">
+        <v>5</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" s="7"/>
+      <c r="E13" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="F13" s="13">
+        <v>0.1681</v>
+      </c>
+      <c r="G13" s="13"/>
+      <c r="H13" s="13">
+        <v>376.1</v>
+      </c>
+      <c r="I13" s="17">
+        <v>63.22</v>
+      </c>
+    </row>
+    <row r="14" ht="14.25" customHeight="1" spans="1:9">
+      <c r="A14" s="6">
+        <v>6</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" s="7"/>
+      <c r="E14" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="F14" s="13">
+        <v>0.001</v>
+      </c>
+      <c r="G14" s="13"/>
+      <c r="H14" s="13">
+        <v>4741.38</v>
+      </c>
+      <c r="I14" s="17">
+        <v>4.74</v>
+      </c>
+    </row>
+    <row r="15" ht="14.25" customHeight="1" spans="1:9">
+      <c r="A15" s="6">
+        <v>7</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D15" s="7"/>
+      <c r="E15" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="F15" s="13">
+        <v>6.0901</v>
+      </c>
+      <c r="G15" s="13"/>
+      <c r="H15" s="13">
+        <v>1</v>
+      </c>
+      <c r="I15" s="17">
+        <v>6.09</v>
+      </c>
+    </row>
+    <row r="16" ht="14.25" customHeight="1" spans="1:9">
+      <c r="A16" s="6">
+        <v>8</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D16" s="7"/>
+      <c r="E16" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="F16" s="13">
+        <v>2.08</v>
+      </c>
+      <c r="G16" s="13"/>
+      <c r="H16" s="13">
+        <v>3.75</v>
+      </c>
+      <c r="I16" s="17">
+        <v>7.8</v>
+      </c>
+    </row>
+    <row r="17" ht="14.25" customHeight="1" spans="1:9">
+      <c r="A17" s="6">
+        <v>9</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D17" s="7"/>
+      <c r="E17" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="F17" s="13">
+        <v>16.74</v>
+      </c>
+      <c r="G17" s="13"/>
+      <c r="H17" s="13">
+        <v>0.07</v>
+      </c>
+      <c r="I17" s="17">
+        <v>1.17</v>
+      </c>
+    </row>
+    <row r="18" ht="14.25" customHeight="1" spans="1:9">
+      <c r="A18" s="6">
+        <v>10</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D18" s="7"/>
+      <c r="E18" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="F18" s="13">
+        <v>0.1899</v>
+      </c>
+      <c r="G18" s="13"/>
+      <c r="H18" s="13">
+        <v>8.74</v>
+      </c>
+      <c r="I18" s="17">
+        <v>1.66</v>
+      </c>
+    </row>
+    <row r="19" ht="14.25" customHeight="1" spans="1:9">
+      <c r="A19" s="6">
+        <v>11</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D19" s="7"/>
+      <c r="E19" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="F19" s="13">
+        <v>1.325</v>
+      </c>
+      <c r="G19" s="13"/>
+      <c r="H19" s="13">
+        <v>101.77</v>
+      </c>
+      <c r="I19" s="17">
+        <v>134.85</v>
+      </c>
+    </row>
+    <row r="20" ht="14.25" customHeight="1" spans="1:9">
+      <c r="A20" s="6"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="13"/>
+      <c r="H20" s="13"/>
+      <c r="I20" s="17"/>
+    </row>
+    <row r="21" ht="14.25" customHeight="1" spans="1:9">
+      <c r="A21" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B21" s="7"/>
+      <c r="C21" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D21" s="7"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="13"/>
+      <c r="H21" s="13"/>
+      <c r="I21" s="17"/>
+    </row>
+    <row r="22" ht="14.25" customHeight="1" spans="1:9">
+      <c r="A22" s="6">
+        <v>1</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="D22" s="7"/>
+      <c r="E22" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="F22" s="13">
+        <v>0.0003</v>
+      </c>
+      <c r="G22" s="13"/>
+      <c r="H22" s="13">
+        <v>464.31</v>
+      </c>
+      <c r="I22" s="17">
+        <v>0.14</v>
+      </c>
+    </row>
+    <row r="23" ht="14.25" customHeight="1" spans="1:9">
+      <c r="A23" s="6">
+        <v>2</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D23" s="7"/>
+      <c r="E23" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="F23" s="13">
+        <v>0.0054</v>
+      </c>
+      <c r="G23" s="13"/>
+      <c r="H23" s="13">
+        <v>217.63</v>
+      </c>
+      <c r="I23" s="17">
+        <v>1.18</v>
+      </c>
+    </row>
+    <row r="24" ht="14.25" customHeight="1" spans="1:9">
+      <c r="A24" s="6">
+        <v>3</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="D24" s="7"/>
+      <c r="E24" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="F24" s="13">
+        <v>0.0189</v>
+      </c>
+      <c r="G24" s="13"/>
+      <c r="H24" s="13">
+        <v>352.72</v>
+      </c>
+      <c r="I24" s="17">
+        <v>6.67</v>
+      </c>
+    </row>
+    <row r="25" ht="14.25" customHeight="1" spans="1:9">
+      <c r="A25" s="6">
+        <v>4</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="D25" s="7"/>
+      <c r="E25" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="F25" s="13">
+        <v>0.0012</v>
+      </c>
+      <c r="G25" s="13"/>
+      <c r="H25" s="13">
+        <v>573.95</v>
+      </c>
+      <c r="I25" s="17">
+        <v>0.69</v>
+      </c>
+    </row>
+    <row r="26" ht="14.25" customHeight="1" spans="1:9">
+      <c r="A26" s="6">
+        <v>5</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="D26" s="7"/>
+      <c r="E26" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="F26" s="13">
+        <v>0.0009</v>
+      </c>
+      <c r="G26" s="13"/>
+      <c r="H26" s="13">
+        <v>555.69</v>
+      </c>
+      <c r="I26" s="17">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="27" ht="14.25" customHeight="1" spans="1:9">
+      <c r="A27" s="6">
+        <v>6</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="D27" s="7"/>
+      <c r="E27" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="F27" s="13">
+        <v>0.0037</v>
+      </c>
+      <c r="G27" s="13"/>
+      <c r="H27" s="13">
+        <v>921.66</v>
+      </c>
+      <c r="I27" s="17">
+        <v>3.41</v>
+      </c>
+    </row>
+    <row r="28" ht="14.25" customHeight="1" spans="1:9">
+      <c r="A28" s="6">
+        <v>7</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="D28" s="7"/>
+      <c r="E28" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="F28" s="13">
+        <v>0.0003</v>
+      </c>
+      <c r="G28" s="13"/>
+      <c r="H28" s="13">
+        <v>324.13</v>
+      </c>
+      <c r="I28" s="17">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="29" ht="14.25" customHeight="1" spans="1:9">
+      <c r="A29" s="6">
+        <v>8</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="D29" s="7"/>
+      <c r="E29" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="F29" s="13">
+        <v>0.0017</v>
+      </c>
+      <c r="G29" s="13"/>
+      <c r="H29" s="13">
+        <v>435.64</v>
+      </c>
+      <c r="I29" s="17">
+        <v>0.74</v>
+      </c>
+    </row>
+    <row r="30" ht="14.25" customHeight="1" spans="1:9">
+      <c r="A30" s="6">
+        <v>9</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="D30" s="7"/>
+      <c r="E30" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="F30" s="13">
+        <v>0.0009</v>
+      </c>
+      <c r="G30" s="13"/>
+      <c r="H30" s="13">
+        <v>231.45</v>
+      </c>
+      <c r="I30" s="17">
+        <v>0.21</v>
+      </c>
+    </row>
+    <row r="31" ht="14.25" customHeight="1" spans="1:9">
+      <c r="A31" s="6">
+        <v>10</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="D31" s="7"/>
+      <c r="E31" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="F31" s="13">
+        <v>0.0024</v>
+      </c>
+      <c r="G31" s="13"/>
+      <c r="H31" s="13">
+        <v>700</v>
+      </c>
+      <c r="I31" s="17">
+        <v>1.68</v>
+      </c>
+    </row>
+    <row r="32" ht="14.25" customHeight="1" spans="1:9">
+      <c r="A32" s="6">
+        <v>11</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="D32" s="7"/>
+      <c r="E32" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="F32" s="13">
+        <v>0.364</v>
+      </c>
+      <c r="G32" s="13"/>
+      <c r="H32" s="13">
+        <v>1</v>
+      </c>
+      <c r="I32" s="17" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="33" ht="14.25" customHeight="1" spans="1:9">
+      <c r="A33" s="6"/>
+      <c r="B33" s="7"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="7"/>
+      <c r="E33" s="12"/>
+      <c r="F33" s="13"/>
+      <c r="G33" s="13"/>
+      <c r="H33" s="13"/>
+      <c r="I33" s="17"/>
+    </row>
+    <row r="34" ht="13.5" customHeight="1" spans="1:9">
+      <c r="A34" s="6"/>
+      <c r="B34" s="7"/>
+      <c r="C34" s="7"/>
+      <c r="D34" s="7"/>
+      <c r="E34" s="12"/>
+      <c r="F34" s="13"/>
+      <c r="G34" s="13"/>
+      <c r="H34" s="13"/>
+      <c r="I34" s="17"/>
+    </row>
+    <row r="35" ht="13.5" customHeight="1" spans="1:9">
+      <c r="A35" s="6"/>
+      <c r="B35" s="7"/>
+      <c r="C35" s="7"/>
+      <c r="D35" s="7"/>
+      <c r="E35" s="12"/>
+      <c r="F35" s="13"/>
+      <c r="G35" s="13"/>
+      <c r="H35" s="13"/>
+      <c r="I35" s="17"/>
+    </row>
+    <row r="36" ht="13.5" customHeight="1" spans="1:9">
+      <c r="A36" s="6"/>
+      <c r="B36" s="7"/>
+      <c r="C36" s="7"/>
+      <c r="D36" s="7"/>
+      <c r="E36" s="12"/>
+      <c r="F36" s="13"/>
+      <c r="G36" s="13"/>
+      <c r="H36" s="13"/>
+      <c r="I36" s="17"/>
+    </row>
+    <row r="37" ht="13.5" customHeight="1" spans="1:9">
+      <c r="A37" s="6"/>
+      <c r="B37" s="7"/>
+      <c r="C37" s="7"/>
+      <c r="D37" s="7"/>
+      <c r="E37" s="12"/>
+      <c r="F37" s="13"/>
+      <c r="G37" s="13"/>
+      <c r="H37" s="13"/>
+      <c r="I37" s="17"/>
+    </row>
+    <row r="38" ht="13.5" customHeight="1" spans="1:9">
+      <c r="A38" s="6"/>
+      <c r="B38" s="7"/>
+      <c r="C38" s="7"/>
+      <c r="D38" s="7"/>
+      <c r="E38" s="12"/>
+      <c r="F38" s="13"/>
+      <c r="G38" s="13"/>
+      <c r="H38" s="13"/>
+      <c r="I38" s="17"/>
+    </row>
+    <row r="39" ht="13.5" customHeight="1" spans="1:9">
+      <c r="A39" s="6"/>
+      <c r="B39" s="7"/>
+      <c r="C39" s="7"/>
+      <c r="D39" s="7"/>
+      <c r="E39" s="12"/>
+      <c r="F39" s="13"/>
+      <c r="G39" s="13"/>
+      <c r="H39" s="13"/>
+      <c r="I39" s="17"/>
+    </row>
+    <row r="40" ht="13.5" customHeight="1" spans="1:9">
+      <c r="A40" s="6"/>
+      <c r="B40" s="7"/>
+      <c r="C40" s="7"/>
+      <c r="D40" s="7"/>
+      <c r="E40" s="12"/>
+      <c r="F40" s="13"/>
+      <c r="G40" s="13"/>
+      <c r="H40" s="13"/>
+      <c r="I40" s="17"/>
+    </row>
+    <row r="41" ht="13.5" customHeight="1" spans="1:9">
+      <c r="A41" s="6"/>
+      <c r="B41" s="7"/>
+      <c r="C41" s="7"/>
+      <c r="D41" s="7"/>
+      <c r="E41" s="12"/>
+      <c r="F41" s="13"/>
+      <c r="G41" s="13"/>
+      <c r="H41" s="13"/>
+      <c r="I41" s="17"/>
+    </row>
+    <row r="42" ht="13.5" customHeight="1" spans="1:9">
+      <c r="A42" s="6"/>
+      <c r="B42" s="7"/>
+      <c r="C42" s="7"/>
+      <c r="D42" s="7"/>
+      <c r="E42" s="12"/>
+      <c r="F42" s="13"/>
+      <c r="G42" s="13"/>
+      <c r="H42" s="13"/>
+      <c r="I42" s="17"/>
+    </row>
+    <row r="43" ht="13.5" customHeight="1" spans="1:9">
+      <c r="A43" s="6"/>
+      <c r="B43" s="7"/>
+      <c r="C43" s="7"/>
+      <c r="D43" s="7"/>
+      <c r="E43" s="12"/>
+      <c r="F43" s="13"/>
+      <c r="G43" s="13"/>
+      <c r="H43" s="13"/>
+      <c r="I43" s="17"/>
+    </row>
+    <row r="44" ht="13.5" customHeight="1" spans="1:9">
+      <c r="A44" s="6"/>
+      <c r="B44" s="7"/>
+      <c r="C44" s="7"/>
+      <c r="D44" s="7"/>
+      <c r="E44" s="12"/>
+      <c r="F44" s="13"/>
+      <c r="G44" s="13"/>
+      <c r="H44" s="13"/>
+      <c r="I44" s="17"/>
+    </row>
+    <row r="45" ht="13.5" customHeight="1" spans="1:9">
+      <c r="A45" s="6"/>
+      <c r="B45" s="7"/>
+      <c r="C45" s="7"/>
+      <c r="D45" s="7"/>
+      <c r="E45" s="12"/>
+      <c r="F45" s="13"/>
+      <c r="G45" s="13"/>
+      <c r="H45" s="13"/>
+      <c r="I45" s="17"/>
+    </row>
+    <row r="46" ht="13.5" customHeight="1" spans="1:9">
+      <c r="A46" s="6"/>
+      <c r="B46" s="7"/>
+      <c r="C46" s="7"/>
+      <c r="D46" s="7"/>
+      <c r="E46" s="12"/>
+      <c r="F46" s="13"/>
+      <c r="G46" s="13"/>
+      <c r="H46" s="13"/>
+      <c r="I46" s="17"/>
+    </row>
+    <row r="47" ht="14.25" customHeight="1" spans="1:9">
+      <c r="A47" s="8"/>
+      <c r="B47" s="9"/>
+      <c r="C47" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="D47" s="9"/>
+      <c r="E47" s="9"/>
+      <c r="F47" s="14"/>
+      <c r="G47" s="14"/>
+      <c r="H47" s="14"/>
+      <c r="I47" s="18">
+        <v>351.6</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="94">
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="F31:G31"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="F32:G32"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="F33:G33"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="F34:G34"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="F35:G35"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="F36:G36"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="F37:G37"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="F38:G38"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="F39:G39"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="F40:G40"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="F43:G43"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="F44:G44"/>
+    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="F45:G45"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="F46:G46"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="F47:G47"/>
+  </mergeCells>
+  <printOptions horizontalCentered="1"/>
+  <pageMargins left="0.303916666666667" right="0.303916666666667" top="0.75" bottom="0" header="0.75" footer="0"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:I47"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="L29" sqref="L29"/>
     </sheetView>
   </sheetViews>
@@ -2467,7 +3484,7 @@
     </row>
     <row r="2" ht="28.5" customHeight="1" spans="1:9">
       <c r="A2" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -3312,7 +4329,1003 @@
       <c r="A47" s="8"/>
       <c r="B47" s="9"/>
       <c r="C47" s="9" t="s">
-        <v>69</v>
+        <v>70</v>
+      </c>
+      <c r="D47" s="9"/>
+      <c r="E47" s="9"/>
+      <c r="F47" s="14"/>
+      <c r="G47" s="14"/>
+      <c r="H47" s="14"/>
+      <c r="I47" s="18">
+        <v>281.67</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="94">
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="F31:G31"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="F32:G32"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="F33:G33"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="F34:G34"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="F35:G35"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="F36:G36"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="F37:G37"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="F38:G38"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="F39:G39"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="F40:G40"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="F43:G43"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="F44:G44"/>
+    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="F45:G45"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="F46:G46"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="F47:G47"/>
+  </mergeCells>
+  <printOptions horizontalCentered="1"/>
+  <pageMargins left="0.303916666666667" right="0.303916666666667" top="0.75" bottom="0" header="0.75" footer="0"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:I47"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="L29" sqref="L29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.6"/>
+  <cols>
+    <col min="1" max="1" width="11.5" customWidth="1"/>
+    <col min="2" max="2" width="14.6590909090909" customWidth="1"/>
+    <col min="3" max="3" width="10.5" customWidth="1"/>
+    <col min="4" max="4" width="20.1590909090909" customWidth="1"/>
+    <col min="5" max="5" width="9.82954545454546" customWidth="1"/>
+    <col min="6" max="6" width="6.5" customWidth="1"/>
+    <col min="7" max="7" width="7.82954545454545" customWidth="1"/>
+    <col min="8" max="9" width="14.3295454545455" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="29.25" customHeight="1" spans="1:9">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+    </row>
+    <row r="2" ht="28.5" customHeight="1" spans="1:9">
+      <c r="A2" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+    </row>
+    <row r="3" ht="14.25" customHeight="1" spans="1:9">
+      <c r="A3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I3" s="15" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" ht="14.25" customHeight="1" spans="1:9">
+      <c r="A4" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="7"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="16"/>
+    </row>
+    <row r="5" ht="14.25" customHeight="1" spans="1:9">
+      <c r="A5" s="6">
+        <v>1</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="7"/>
+      <c r="E5" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="13">
+        <v>0.0877</v>
+      </c>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13">
+        <v>118.5</v>
+      </c>
+      <c r="I5" s="17">
+        <v>10.39</v>
+      </c>
+    </row>
+    <row r="6" ht="14.25" customHeight="1" spans="1:9">
+      <c r="A6" s="6">
+        <v>2</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="7"/>
+      <c r="E6" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" s="13">
+        <v>-0.0003</v>
+      </c>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13">
+        <v>1</v>
+      </c>
+      <c r="I6" s="17"/>
+    </row>
+    <row r="7" ht="14.25" customHeight="1" spans="1:9">
+      <c r="A7" s="6"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="17"/>
+    </row>
+    <row r="8" ht="14.25" customHeight="1" spans="1:9">
+      <c r="A8" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="7"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="17"/>
+    </row>
+    <row r="9" ht="14.25" customHeight="1" spans="1:9">
+      <c r="A9" s="6">
+        <v>1</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="7"/>
+      <c r="E9" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="F9" s="13">
+        <v>-0.0003</v>
+      </c>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13">
+        <v>1</v>
+      </c>
+      <c r="I9" s="17"/>
+    </row>
+    <row r="10" ht="14.25" customHeight="1" spans="1:9">
+      <c r="A10" s="6">
+        <v>2</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="7"/>
+      <c r="E10" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="F10" s="13">
+        <v>1.1715</v>
+      </c>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13">
+        <v>7.76</v>
+      </c>
+      <c r="I10" s="17">
+        <v>9.09</v>
+      </c>
+    </row>
+    <row r="11" ht="14.25" customHeight="1" spans="1:9">
+      <c r="A11" s="6">
+        <v>3</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" s="7"/>
+      <c r="E11" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="F11" s="13">
+        <v>0.0938</v>
+      </c>
+      <c r="G11" s="13"/>
+      <c r="H11" s="13">
+        <v>402.7</v>
+      </c>
+      <c r="I11" s="17">
+        <v>37.77</v>
+      </c>
+    </row>
+    <row r="12" ht="14.25" customHeight="1" spans="1:9">
+      <c r="A12" s="6">
+        <v>4</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" s="7"/>
+      <c r="E12" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="F12" s="13">
+        <v>0.1681</v>
+      </c>
+      <c r="G12" s="13"/>
+      <c r="H12" s="13">
+        <v>376.1</v>
+      </c>
+      <c r="I12" s="17">
+        <v>63.22</v>
+      </c>
+    </row>
+    <row r="13" ht="14.25" customHeight="1" spans="1:9">
+      <c r="A13" s="6">
+        <v>5</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" s="7"/>
+      <c r="E13" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="F13" s="13">
+        <v>0.001</v>
+      </c>
+      <c r="G13" s="13"/>
+      <c r="H13" s="13">
+        <v>4741.38</v>
+      </c>
+      <c r="I13" s="17">
+        <v>4.74</v>
+      </c>
+    </row>
+    <row r="14" ht="14.25" customHeight="1" spans="1:9">
+      <c r="A14" s="6">
+        <v>6</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D14" s="7"/>
+      <c r="E14" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="F14" s="13">
+        <v>4.9224</v>
+      </c>
+      <c r="G14" s="13"/>
+      <c r="H14" s="13">
+        <v>1</v>
+      </c>
+      <c r="I14" s="17">
+        <v>4.92</v>
+      </c>
+    </row>
+    <row r="15" ht="14.25" customHeight="1" spans="1:9">
+      <c r="A15" s="6">
+        <v>7</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D15" s="7"/>
+      <c r="E15" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="F15" s="13">
+        <v>1.56</v>
+      </c>
+      <c r="G15" s="13"/>
+      <c r="H15" s="13">
+        <v>3.75</v>
+      </c>
+      <c r="I15" s="17">
+        <v>5.85</v>
+      </c>
+    </row>
+    <row r="16" ht="14.25" customHeight="1" spans="1:9">
+      <c r="A16" s="6">
+        <v>8</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D16" s="7"/>
+      <c r="E16" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="F16" s="13">
+        <v>16.74</v>
+      </c>
+      <c r="G16" s="13"/>
+      <c r="H16" s="13">
+        <v>0.07</v>
+      </c>
+      <c r="I16" s="17">
+        <v>1.17</v>
+      </c>
+    </row>
+    <row r="17" ht="14.25" customHeight="1" spans="1:9">
+      <c r="A17" s="6">
+        <v>9</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D17" s="7"/>
+      <c r="E17" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="F17" s="13">
+        <v>0.1833</v>
+      </c>
+      <c r="G17" s="13"/>
+      <c r="H17" s="13">
+        <v>8.74</v>
+      </c>
+      <c r="I17" s="17">
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="18" ht="14.25" customHeight="1" spans="1:9">
+      <c r="A18" s="6">
+        <v>10</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D18" s="7"/>
+      <c r="E18" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="F18" s="13">
+        <v>1.272</v>
+      </c>
+      <c r="G18" s="13"/>
+      <c r="H18" s="13">
+        <v>101.77</v>
+      </c>
+      <c r="I18" s="17">
+        <v>129.45</v>
+      </c>
+    </row>
+    <row r="19" ht="14.25" customHeight="1" spans="1:9">
+      <c r="A19" s="6"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
+      <c r="H19" s="13"/>
+      <c r="I19" s="17"/>
+    </row>
+    <row r="20" ht="14.25" customHeight="1" spans="1:9">
+      <c r="A20" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B20" s="7"/>
+      <c r="C20" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D20" s="7"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="13"/>
+      <c r="H20" s="13"/>
+      <c r="I20" s="17"/>
+    </row>
+    <row r="21" ht="14.25" customHeight="1" spans="1:9">
+      <c r="A21" s="6">
+        <v>1</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="D21" s="7"/>
+      <c r="E21" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="F21" s="13">
+        <v>0.0003</v>
+      </c>
+      <c r="G21" s="13"/>
+      <c r="H21" s="13">
+        <v>464.31</v>
+      </c>
+      <c r="I21" s="17">
+        <v>0.14</v>
+      </c>
+    </row>
+    <row r="22" ht="14.25" customHeight="1" spans="1:9">
+      <c r="A22" s="6">
+        <v>2</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D22" s="7"/>
+      <c r="E22" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="F22" s="13">
+        <v>0.0054</v>
+      </c>
+      <c r="G22" s="13"/>
+      <c r="H22" s="13">
+        <v>217.63</v>
+      </c>
+      <c r="I22" s="17">
+        <v>1.18</v>
+      </c>
+    </row>
+    <row r="23" ht="14.25" customHeight="1" spans="1:9">
+      <c r="A23" s="6">
+        <v>3</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="D23" s="7"/>
+      <c r="E23" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="F23" s="13">
+        <v>0.0156</v>
+      </c>
+      <c r="G23" s="13"/>
+      <c r="H23" s="13">
+        <v>352.72</v>
+      </c>
+      <c r="I23" s="17">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="24" ht="14.25" customHeight="1" spans="1:9">
+      <c r="A24" s="6">
+        <v>4</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="D24" s="7"/>
+      <c r="E24" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="F24" s="13">
+        <v>0.0012</v>
+      </c>
+      <c r="G24" s="13"/>
+      <c r="H24" s="13">
+        <v>573.95</v>
+      </c>
+      <c r="I24" s="17">
+        <v>0.69</v>
+      </c>
+    </row>
+    <row r="25" ht="14.25" customHeight="1" spans="1:9">
+      <c r="A25" s="6">
+        <v>5</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="D25" s="7"/>
+      <c r="E25" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="F25" s="13">
+        <v>0.0009</v>
+      </c>
+      <c r="G25" s="13"/>
+      <c r="H25" s="13">
+        <v>555.69</v>
+      </c>
+      <c r="I25" s="17">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="26" ht="14.25" customHeight="1" spans="1:9">
+      <c r="A26" s="6">
+        <v>6</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="D26" s="7"/>
+      <c r="E26" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="F26" s="13">
+        <v>0.0029</v>
+      </c>
+      <c r="G26" s="13"/>
+      <c r="H26" s="13">
+        <v>921.66</v>
+      </c>
+      <c r="I26" s="17">
+        <v>2.67</v>
+      </c>
+    </row>
+    <row r="27" ht="14.25" customHeight="1" spans="1:9">
+      <c r="A27" s="6">
+        <v>7</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="D27" s="7"/>
+      <c r="E27" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="F27" s="13">
+        <v>0.0003</v>
+      </c>
+      <c r="G27" s="13"/>
+      <c r="H27" s="13">
+        <v>324.13</v>
+      </c>
+      <c r="I27" s="17">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="28" ht="14.25" customHeight="1" spans="1:9">
+      <c r="A28" s="6">
+        <v>8</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="D28" s="7"/>
+      <c r="E28" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="F28" s="13">
+        <v>0.0012</v>
+      </c>
+      <c r="G28" s="13"/>
+      <c r="H28" s="13">
+        <v>435.64</v>
+      </c>
+      <c r="I28" s="17">
+        <v>0.52</v>
+      </c>
+    </row>
+    <row r="29" ht="14.25" customHeight="1" spans="1:9">
+      <c r="A29" s="6">
+        <v>9</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="D29" s="7"/>
+      <c r="E29" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="F29" s="13">
+        <v>0.0009</v>
+      </c>
+      <c r="G29" s="13"/>
+      <c r="H29" s="13">
+        <v>231.45</v>
+      </c>
+      <c r="I29" s="17">
+        <v>0.21</v>
+      </c>
+    </row>
+    <row r="30" ht="14.25" customHeight="1" spans="1:9">
+      <c r="A30" s="6">
+        <v>10</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="D30" s="7"/>
+      <c r="E30" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="F30" s="13">
+        <v>0.0024</v>
+      </c>
+      <c r="G30" s="13"/>
+      <c r="H30" s="13">
+        <v>700</v>
+      </c>
+      <c r="I30" s="17">
+        <v>1.68</v>
+      </c>
+    </row>
+    <row r="31" ht="14.25" customHeight="1" spans="1:9">
+      <c r="A31" s="6">
+        <v>11</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="D31" s="7"/>
+      <c r="E31" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="F31" s="13">
+        <v>0.2842</v>
+      </c>
+      <c r="G31" s="13"/>
+      <c r="H31" s="13">
+        <v>1</v>
+      </c>
+      <c r="I31" s="17">
+        <v>0.28</v>
+      </c>
+    </row>
+    <row r="32" ht="14.25" customHeight="1" spans="1:9">
+      <c r="A32" s="6"/>
+      <c r="B32" s="7"/>
+      <c r="C32" s="7"/>
+      <c r="D32" s="7"/>
+      <c r="E32" s="12"/>
+      <c r="F32" s="13"/>
+      <c r="G32" s="13"/>
+      <c r="H32" s="13"/>
+      <c r="I32" s="17"/>
+    </row>
+    <row r="33" ht="13.5" customHeight="1" spans="1:9">
+      <c r="A33" s="6"/>
+      <c r="B33" s="7"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="7"/>
+      <c r="E33" s="12"/>
+      <c r="F33" s="13"/>
+      <c r="G33" s="13"/>
+      <c r="H33" s="13"/>
+      <c r="I33" s="17"/>
+    </row>
+    <row r="34" ht="13.5" customHeight="1" spans="1:9">
+      <c r="A34" s="6"/>
+      <c r="B34" s="7"/>
+      <c r="C34" s="7"/>
+      <c r="D34" s="7"/>
+      <c r="E34" s="12"/>
+      <c r="F34" s="13"/>
+      <c r="G34" s="13"/>
+      <c r="H34" s="13"/>
+      <c r="I34" s="17"/>
+    </row>
+    <row r="35" ht="13.5" customHeight="1" spans="1:9">
+      <c r="A35" s="6"/>
+      <c r="B35" s="7"/>
+      <c r="C35" s="7"/>
+      <c r="D35" s="7"/>
+      <c r="E35" s="12"/>
+      <c r="F35" s="13"/>
+      <c r="G35" s="13"/>
+      <c r="H35" s="13"/>
+      <c r="I35" s="17"/>
+    </row>
+    <row r="36" ht="13.5" customHeight="1" spans="1:9">
+      <c r="A36" s="6"/>
+      <c r="B36" s="7"/>
+      <c r="C36" s="7"/>
+      <c r="D36" s="7"/>
+      <c r="E36" s="12"/>
+      <c r="F36" s="13"/>
+      <c r="G36" s="13"/>
+      <c r="H36" s="13"/>
+      <c r="I36" s="17"/>
+    </row>
+    <row r="37" ht="13.5" customHeight="1" spans="1:9">
+      <c r="A37" s="6"/>
+      <c r="B37" s="7"/>
+      <c r="C37" s="7"/>
+      <c r="D37" s="7"/>
+      <c r="E37" s="12"/>
+      <c r="F37" s="13"/>
+      <c r="G37" s="13"/>
+      <c r="H37" s="13"/>
+      <c r="I37" s="17"/>
+    </row>
+    <row r="38" ht="13.5" customHeight="1" spans="1:9">
+      <c r="A38" s="6"/>
+      <c r="B38" s="7"/>
+      <c r="C38" s="7"/>
+      <c r="D38" s="7"/>
+      <c r="E38" s="12"/>
+      <c r="F38" s="13"/>
+      <c r="G38" s="13"/>
+      <c r="H38" s="13"/>
+      <c r="I38" s="17"/>
+    </row>
+    <row r="39" ht="13.5" customHeight="1" spans="1:9">
+      <c r="A39" s="6"/>
+      <c r="B39" s="7"/>
+      <c r="C39" s="7"/>
+      <c r="D39" s="7"/>
+      <c r="E39" s="12"/>
+      <c r="F39" s="13"/>
+      <c r="G39" s="13"/>
+      <c r="H39" s="13"/>
+      <c r="I39" s="17"/>
+    </row>
+    <row r="40" ht="13.5" customHeight="1" spans="1:9">
+      <c r="A40" s="6"/>
+      <c r="B40" s="7"/>
+      <c r="C40" s="7"/>
+      <c r="D40" s="7"/>
+      <c r="E40" s="12"/>
+      <c r="F40" s="13"/>
+      <c r="G40" s="13"/>
+      <c r="H40" s="13"/>
+      <c r="I40" s="17"/>
+    </row>
+    <row r="41" ht="13.5" customHeight="1" spans="1:9">
+      <c r="A41" s="6"/>
+      <c r="B41" s="7"/>
+      <c r="C41" s="7"/>
+      <c r="D41" s="7"/>
+      <c r="E41" s="12"/>
+      <c r="F41" s="13"/>
+      <c r="G41" s="13"/>
+      <c r="H41" s="13"/>
+      <c r="I41" s="17"/>
+    </row>
+    <row r="42" ht="13.5" customHeight="1" spans="1:9">
+      <c r="A42" s="6"/>
+      <c r="B42" s="7"/>
+      <c r="C42" s="7"/>
+      <c r="D42" s="7"/>
+      <c r="E42" s="12"/>
+      <c r="F42" s="13"/>
+      <c r="G42" s="13"/>
+      <c r="H42" s="13"/>
+      <c r="I42" s="17"/>
+    </row>
+    <row r="43" ht="13.5" customHeight="1" spans="1:9">
+      <c r="A43" s="6"/>
+      <c r="B43" s="7"/>
+      <c r="C43" s="7"/>
+      <c r="D43" s="7"/>
+      <c r="E43" s="12"/>
+      <c r="F43" s="13"/>
+      <c r="G43" s="13"/>
+      <c r="H43" s="13"/>
+      <c r="I43" s="17"/>
+    </row>
+    <row r="44" ht="13.5" customHeight="1" spans="1:9">
+      <c r="A44" s="6"/>
+      <c r="B44" s="7"/>
+      <c r="C44" s="7"/>
+      <c r="D44" s="7"/>
+      <c r="E44" s="12"/>
+      <c r="F44" s="13"/>
+      <c r="G44" s="13"/>
+      <c r="H44" s="13"/>
+      <c r="I44" s="17"/>
+    </row>
+    <row r="45" ht="13.5" customHeight="1" spans="1:9">
+      <c r="A45" s="6"/>
+      <c r="B45" s="7"/>
+      <c r="C45" s="7"/>
+      <c r="D45" s="7"/>
+      <c r="E45" s="12"/>
+      <c r="F45" s="13"/>
+      <c r="G45" s="13"/>
+      <c r="H45" s="13"/>
+      <c r="I45" s="17"/>
+    </row>
+    <row r="46" ht="13.5" customHeight="1" spans="1:9">
+      <c r="A46" s="6"/>
+      <c r="B46" s="7"/>
+      <c r="C46" s="7"/>
+      <c r="D46" s="7"/>
+      <c r="E46" s="12"/>
+      <c r="F46" s="13"/>
+      <c r="G46" s="13"/>
+      <c r="H46" s="13"/>
+      <c r="I46" s="17"/>
+    </row>
+    <row r="47" ht="14.25" customHeight="1" spans="1:9">
+      <c r="A47" s="8"/>
+      <c r="B47" s="9"/>
+      <c r="C47" s="9" t="s">
+        <v>70</v>
       </c>
       <c r="D47" s="9"/>
       <c r="E47" s="9"/>

</xml_diff>